<commit_message>
new endpoints for wp
</commit_message>
<xml_diff>
--- a/application/upload/new_disciplines_test_bachelor_3 (1)_small.xlsx
+++ b/application/upload/new_disciplines_test_bachelor_3 (1)_small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tonik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8EC835-9235-4A65-823B-403328B843DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB3F11E-AB82-46C4-BDD2-26F6A963DBC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$15224</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$14817</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>SUBFIELDCODE</t>
   </si>
@@ -64,112 +64,61 @@
     <t>TYPELEARNING</t>
   </si>
   <si>
+    <t>09.03.03</t>
+  </si>
+  <si>
+    <t>Прикладная информатика</t>
+  </si>
+  <si>
+    <t>Мобильные и сетевые технологии</t>
+  </si>
+  <si>
+    <t>Академический бакалавр</t>
+  </si>
+  <si>
+    <t>Блок 1. Модули (дисциплины)</t>
+  </si>
+  <si>
+    <t>Универсальный модуль</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>традиционное</t>
+  </si>
+  <si>
+    <t>06.0.0.0.18</t>
+  </si>
+  <si>
+    <t>06.0.0.1.18</t>
+  </si>
+  <si>
+    <t>06.0.0.2.18</t>
+  </si>
+  <si>
     <t>DIS_CODE</t>
   </si>
   <si>
-    <t>01.03.02</t>
-  </si>
-  <si>
-    <t>Прикладная математика и информатика</t>
-  </si>
-  <si>
-    <t>Информатика и программирование</t>
-  </si>
-  <si>
-    <t>Академический бакалавр</t>
-  </si>
-  <si>
-    <t>История</t>
-  </si>
-  <si>
-    <t>Безопасность жизнедеятельности</t>
-  </si>
-  <si>
-    <t>Физическая культура</t>
-  </si>
-  <si>
-    <t>Философия</t>
-  </si>
-  <si>
-    <t>Введение в цифровую культуру и программирование</t>
-  </si>
-  <si>
-    <t>Проектирование баз данных</t>
-  </si>
-  <si>
-    <t>Математическая статистика</t>
-  </si>
-  <si>
-    <t>Машинное обучение</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Современные вопросы информатики </t>
-  </si>
-  <si>
-    <t>Анализ данных и информационный поиск</t>
-  </si>
-  <si>
-    <t>Психология предпринимательства</t>
-  </si>
-  <si>
-    <t>Блок 1. Модули (дисциплины)</t>
-  </si>
-  <si>
-    <t>Универсальный модуль</t>
-  </si>
-  <si>
-    <t>Модуль «Философия+Мышление»</t>
-  </si>
-  <si>
-    <t>Модуль «Цифровая культура»</t>
-  </si>
-  <si>
-    <t>Модуль «Предпринимательская культура»</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Optionally</t>
-  </si>
-  <si>
-    <t>традиционное</t>
-  </si>
-  <si>
-    <t>смешанное</t>
-  </si>
-  <si>
-    <t>06.0.0.0.18</t>
-  </si>
-  <si>
-    <t>06.0.0.1.18</t>
-  </si>
-  <si>
-    <t>06.0.0.2.18</t>
-  </si>
-  <si>
-    <t>06.0.1.0.18</t>
-  </si>
-  <si>
-    <t>06.0.2.0.18</t>
-  </si>
-  <si>
-    <t>06.0.2.1.18</t>
-  </si>
-  <si>
-    <t>06.0.2.2.18</t>
-  </si>
-  <si>
-    <t>06.0.2.3.18</t>
-  </si>
-  <si>
-    <t>06.0.2.4.18</t>
-  </si>
-  <si>
-    <t>06.0.2.5.18</t>
-  </si>
-  <si>
-    <t>06.0.4.0.18</t>
+    <t>История11122</t>
+  </si>
+  <si>
+    <t>Физическая культура11122</t>
+  </si>
+  <si>
+    <t>Безопасность жизнедеятельности12211</t>
+  </si>
+  <si>
+    <t>История11111222</t>
+  </si>
+  <si>
+    <t>Безопасность жизнедеятельности122222211</t>
+  </si>
+  <si>
+    <t>Физическая культура11122222</t>
+  </si>
+  <si>
+    <t>Мобильные и сетевые технологии 222</t>
   </si>
 </sst>
 </file>
@@ -571,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,6 +531,7 @@
     <col min="2" max="2" width="36.33203125" customWidth="1"/>
     <col min="3" max="3" width="49.44140625" customWidth="1"/>
     <col min="7" max="7" width="32.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
     <col min="13" max="13" width="25.77734375" customWidth="1"/>
     <col min="14" max="14" width="23.6640625" customWidth="1"/>
   </cols>
@@ -627,539 +577,266 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2">
         <v>2018</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3">
+        <v>2019</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="D3">
-        <v>2018</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4">
+        <v>2020</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4">
-        <v>2018</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>2018</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
         <v>20</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>2019</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
-        <v>2018</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
         <v>17</v>
       </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6">
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
         <v>3</v>
       </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6">
-        <v>6</v>
-      </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>2020</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
-        <v>2018</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <v>2018</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8">
-        <v>7</v>
-      </c>
-      <c r="L8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>2018</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9">
-        <v>4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9">
-        <v>5</v>
-      </c>
-      <c r="L9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" t="s">
-        <v>36</v>
-      </c>
-      <c r="N9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>2018</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10">
-        <v>6</v>
-      </c>
-      <c r="L10" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>2018</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11">
-        <v>6</v>
-      </c>
-      <c r="I11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11">
-        <v>7</v>
-      </c>
-      <c r="L11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12">
-        <v>2018</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12">
-        <v>8</v>
-      </c>
-      <c r="L12" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>2018</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13">
-        <v>6</v>
-      </c>
-      <c r="L13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N15224" xr:uid="{33A2569A-28B4-49A3-8F36-B3E3B3D9CF8A}"/>
+  <autoFilter ref="A1:N14817" xr:uid="{33A2569A-28B4-49A3-8F36-B3E3B3D9CF8A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>